<commit_message>
Edit Log Book dan Burn Down Chart
</commit_message>
<xml_diff>
--- a/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
+++ b/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
@@ -316,7 +316,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="id-ID"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -325,7 +325,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr lang="en-US"/>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -347,6 +347,16 @@
             <c:v>Ideal burndown</c:v>
           </c:tx>
           <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US"/>
+                </a:pPr>
+                <a:endParaRPr lang="id-ID"/>
+              </a:p>
+            </c:txPr>
             <c:showVal val="1"/>
           </c:dLbls>
           <c:cat>
@@ -434,6 +444,16 @@
             <c:v>Actual burndown</c:v>
           </c:tx>
           <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US"/>
+                </a:pPr>
+                <a:endParaRPr lang="id-ID"/>
+              </a:p>
+            </c:txPr>
             <c:showVal val="1"/>
           </c:dLbls>
           <c:cat>
@@ -503,25 +523,35 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="57404416"/>
-        <c:axId val="67572480"/>
+        <c:axId val="80788096"/>
+        <c:axId val="81002880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57404416"/>
+        <c:axId val="80788096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67572480"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="id-ID"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="81002880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67572480"/>
+        <c:axId val="81002880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,7 +559,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="57404416"/>
+        <c:crossAx val="80788096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -537,12 +567,22 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US"/>
+          </a:pPr>
+          <a:endParaRPr lang="id-ID"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -870,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -878,7 +918,7 @@
   <cols>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" s="5" customFormat="1" ht="15.75">

</xml_diff>

<commit_message>
tambah dolphin albino, tambah gambar dolphin,tiger,lion,aligator,snake albino, rapikan slide mengidentifikasi albino, rapikan bagian mitos albino
</commit_message>
<xml_diff>
--- a/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
+++ b/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Project</t>
   </si>
@@ -76,78 +76,6 @@
   </si>
   <si>
     <t>Start</t>
-  </si>
-  <si>
-    <t>Day 10</t>
-  </si>
-  <si>
-    <t>Day 9</t>
-  </si>
-  <si>
-    <t>Day 8</t>
-  </si>
-  <si>
-    <t>Day 7</t>
-  </si>
-  <si>
-    <t>Day 6</t>
-  </si>
-  <si>
-    <t>Day 5</t>
-  </si>
-  <si>
-    <t>Day 4</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
-    <t>Day 2</t>
-  </si>
-  <si>
-    <t>Day 1</t>
-  </si>
-  <si>
-    <t>My Project</t>
-  </si>
-  <si>
-    <t>Story 1</t>
-  </si>
-  <si>
-    <t>Story 2</t>
-  </si>
-  <si>
-    <t>Story 3</t>
-  </si>
-  <si>
-    <t>Story 4</t>
-  </si>
-  <si>
-    <t>Task 2.2</t>
-  </si>
-  <si>
-    <t>Task 3.1</t>
-  </si>
-  <si>
-    <t>Task 3.2</t>
-  </si>
-  <si>
-    <t>Task 3.3</t>
-  </si>
-  <si>
-    <t>Task 3.4</t>
-  </si>
-  <si>
-    <t>Task 4.1</t>
-  </si>
-  <si>
-    <t>Task 4.2</t>
-  </si>
-  <si>
-    <t>Task 4.3</t>
-  </si>
-  <si>
-    <t>Task 4.4</t>
   </si>
   <si>
     <t>Ideal - Remaining efforts in uninterrupted working hours</t>
@@ -162,19 +90,67 @@
     <t>www.goodoldmanoj.com</t>
   </si>
   <si>
-    <t>Penyembuhan albino</t>
+    <t>Pengenalan Albino</t>
   </si>
   <si>
-    <t>Gejala albino</t>
+    <t>Albino</t>
   </si>
   <si>
-    <t>Penyebab albino</t>
+    <t>Pengertian Albino</t>
   </si>
   <si>
-    <t>Pengertian albino</t>
+    <t>Penyebab Albino</t>
   </si>
   <si>
-    <t>Pengenalan Albino</t>
+    <t>Gejala Albino</t>
+  </si>
+  <si>
+    <t>Penyembuhan Albino</t>
+  </si>
+  <si>
+    <t>Kategori Albino</t>
+  </si>
+  <si>
+    <t>Albino Tirosinase Positif</t>
+  </si>
+  <si>
+    <t>Albino Tirosinase Negatif</t>
+  </si>
+  <si>
+    <t>Tipe Albino</t>
+  </si>
+  <si>
+    <t>Oculocutaneous Albinism</t>
+  </si>
+  <si>
+    <t>Ocular Albinism</t>
+  </si>
+  <si>
+    <t>Mitos Albino</t>
+  </si>
+  <si>
+    <t>Mitos Albino Pada Manusia</t>
+  </si>
+  <si>
+    <t>Albino Pada Hewan</t>
+  </si>
+  <si>
+    <t>Pengantar Albino Pada Hewan</t>
+  </si>
+  <si>
+    <t>Mengidentifikasi Albino Pada Hewan</t>
+  </si>
+  <si>
+    <t>Masalah Pada Hewan Albino</t>
+  </si>
+  <si>
+    <t>Mitos Albino Pada Hewan</t>
+  </si>
+  <si>
+    <t>Hewan Albino Terindah</t>
+  </si>
+  <si>
+    <t>9 Hewan Albino Terindah</t>
   </si>
 </sst>
 </file>
@@ -278,12 +254,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
@@ -294,6 +267,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -360,78 +341,79 @@
             <c:showVal val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$F$5:$O$5</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>dd\-mmm</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Day 10</c:v>
+                  <c:v>41785</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Day 9</c:v>
+                  <c:v>41786</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Day 8</c:v>
+                  <c:v>41787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Day 7</c:v>
+                  <c:v>41788</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Day 6</c:v>
+                  <c:v>41789</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Day 5</c:v>
+                  <c:v>41790</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Day 4</c:v>
+                  <c:v>41792</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Day 3</c:v>
+                  <c:v>41793</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Day 2</c:v>
+                  <c:v>41794</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Day 1</c:v>
+                  <c:v>41795</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$19:$O$19</c:f>
+              <c:f>Sheet1!$F$28:$O$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>67.5</c:v>
+                  <c:v>51.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>45.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.5</c:v>
+                  <c:v>39.899999999999991</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>34.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.5</c:v>
+                  <c:v>28.499999999999989</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>22.79999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.5</c:v>
+                  <c:v>17.099999999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>11.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.5</c:v>
+                  <c:v>5.6999999999999913</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>-8.8817841970012523E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,63 +439,64 @@
             <c:showVal val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$F$5:$O$5</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>dd\-mmm</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Day 10</c:v>
+                  <c:v>41785</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Day 9</c:v>
+                  <c:v>41786</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Day 8</c:v>
+                  <c:v>41787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Day 7</c:v>
+                  <c:v>41788</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Day 6</c:v>
+                  <c:v>41789</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Day 5</c:v>
+                  <c:v>41790</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Day 4</c:v>
+                  <c:v>41792</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Day 3</c:v>
+                  <c:v>41793</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Day 2</c:v>
+                  <c:v>41794</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Day 1</c:v>
+                  <c:v>41795</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$20:$O$20</c:f>
+              <c:f>Sheet1!$F$29:$O$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>74</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -523,15 +506,16 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="80788096"/>
-        <c:axId val="81002880"/>
+        <c:axId val="70381952"/>
+        <c:axId val="70383488"/>
       </c:lineChart>
-      <c:catAx>
-        <c:axId val="80788096"/>
+      <c:dateAx>
+        <c:axId val="70381952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -544,14 +528,13 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81002880"/>
+        <c:crossAx val="70383488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-      </c:catAx>
+      </c:dateAx>
       <c:valAx>
-        <c:axId val="81002880"/>
+        <c:axId val="70383488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +542,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="80788096"/>
+        <c:crossAx val="70381952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -582,7 +565,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -594,13 +577,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>514351</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -908,30 +891,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD56"/>
+  <dimension ref="A1:XFC65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="5" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16383" s="4" customFormat="1" ht="15.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="9" t="s">
-        <v>31</v>
+      <c r="E1" s="10" t="s">
+        <v>7</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -17307,9 +17291,8 @@
       <c r="XFA1" s="1"/>
       <c r="XFB1" s="1"/>
       <c r="XFC1" s="1"/>
-      <c r="XFD1" s="1"/>
     </row>
-    <row r="2" spans="1:16384" s="6" customFormat="1" ht="17.25" customHeight="1">
+    <row r="2" spans="1:16383" s="5" customFormat="1" ht="17.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -33693,20 +33676,19 @@
       <c r="XFA2" s="1"/>
       <c r="XFB2" s="1"/>
       <c r="XFC2" s="1"/>
-      <c r="XFD2" s="1"/>
     </row>
-    <row r="3" spans="1:16384" s="5" customFormat="1" ht="23.25">
+    <row r="3" spans="1:16383" s="4" customFormat="1" ht="23.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="8" t="s">
-        <v>30</v>
+      <c r="D3" s="9" t="s">
+        <v>6</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -50081,9 +50063,8 @@
       <c r="XFA3" s="1"/>
       <c r="XFB3" s="1"/>
       <c r="XFC3" s="1"/>
-      <c r="XFD3" s="1"/>
     </row>
-    <row r="4" spans="1:16384">
+    <row r="4" spans="1:16383">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -50104,839 +50085,711 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:16384">
+    <row r="5" spans="1:16383">
       <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>4</v>
+      <c r="F5" s="7">
+        <v>41785</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>5</v>
+      <c r="G5" s="7">
+        <v>41786</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>6</v>
+      <c r="H5" s="7">
+        <v>41787</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>7</v>
+      <c r="I5" s="7">
+        <v>41788</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>8</v>
+      <c r="J5" s="7">
+        <v>41789</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>9</v>
+      <c r="K5" s="7">
+        <v>41790</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>10</v>
+      <c r="L5" s="7">
+        <v>41792</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>11</v>
+      <c r="M5" s="7">
+        <v>41793</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>12</v>
+      <c r="N5" s="7">
+        <v>41794</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>13</v>
+      <c r="O5" s="7">
+        <v>41795</v>
       </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="P5" s="7">
+        <v>41796</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>41797</v>
+      </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:16384">
+    <row r="6" spans="1:16383">
       <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
-        <v>36</v>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>35</v>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
       </c>
-      <c r="E6" s="4">
-        <v>3</v>
-      </c>
-      <c r="F6" s="4">
-        <v>3</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:16384">
+    <row r="7" spans="1:16383">
       <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="4">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4">
-        <v>3</v>
-      </c>
-      <c r="G7" s="4">
-        <v>3</v>
-      </c>
-      <c r="H7" s="4">
-        <v>5</v>
-      </c>
-      <c r="I7" s="4">
-        <v>2</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:16384">
+    <row r="8" spans="1:16383">
       <c r="A8" s="1"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>33</v>
+      <c r="E8" s="3">
+        <v>10</v>
       </c>
-      <c r="E8" s="4">
-        <v>3</v>
+      <c r="F8" s="3">
+        <v>8</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="3">
+        <v>6</v>
+      </c>
+      <c r="H8" s="3">
         <v>2</v>
       </c>
-      <c r="G8" s="4">
-        <v>3</v>
-      </c>
-      <c r="H8" s="4">
-        <v>2</v>
-      </c>
-      <c r="I8" s="4">
-        <v>2</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:16384">
+    <row r="9" spans="1:16383">
       <c r="A9" s="1"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>32</v>
+      <c r="E9" s="3">
+        <v>8</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="3">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3">
         <v>3</v>
       </c>
-      <c r="F9" s="4">
-        <v>3</v>
+      <c r="H9" s="3">
+        <v>1</v>
       </c>
-      <c r="G9" s="4">
-        <v>8</v>
-      </c>
-      <c r="H9" s="4">
-        <v>8</v>
-      </c>
-      <c r="I9" s="4">
-        <v>7</v>
-      </c>
-      <c r="J9" s="4">
-        <v>3</v>
-      </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:16384">
+    <row r="10" spans="1:16383">
       <c r="A10" s="1"/>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="4">
-        <v>8</v>
-      </c>
-      <c r="F10" s="4">
-        <v>8</v>
-      </c>
-      <c r="G10" s="4">
-        <v>8</v>
-      </c>
-      <c r="H10" s="4">
-        <v>8</v>
-      </c>
-      <c r="I10" s="4">
-        <v>8</v>
-      </c>
-      <c r="J10" s="4">
-        <v>7</v>
-      </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:16384">
+    <row r="11" spans="1:16383">
       <c r="A11" s="1"/>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="4">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4">
-        <v>9</v>
-      </c>
-      <c r="G11" s="4">
-        <v>9</v>
-      </c>
-      <c r="H11" s="4">
-        <v>9</v>
-      </c>
-      <c r="I11" s="4">
-        <v>9</v>
-      </c>
-      <c r="J11" s="4">
-        <v>9</v>
-      </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:16384">
+    <row r="12" spans="1:16383">
       <c r="A12" s="1"/>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>21</v>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
       </c>
-      <c r="E12" s="4">
-        <v>5</v>
-      </c>
-      <c r="F12" s="4">
-        <v>5</v>
-      </c>
-      <c r="G12" s="4">
-        <v>5</v>
-      </c>
-      <c r="H12" s="4">
-        <v>5</v>
-      </c>
-      <c r="I12" s="4">
-        <v>5</v>
-      </c>
-      <c r="J12" s="4">
-        <v>5</v>
-      </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:16384">
+    <row r="13" spans="1:16383">
       <c r="A13" s="1"/>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>7</v>
       </c>
-      <c r="F13" s="4">
-        <v>7</v>
+      <c r="F13" s="3">
+        <v>5</v>
       </c>
-      <c r="G13" s="4">
-        <v>7</v>
+      <c r="G13" s="3">
+        <v>2</v>
       </c>
-      <c r="H13" s="4">
-        <v>7</v>
+      <c r="H13" s="3">
+        <v>1</v>
       </c>
-      <c r="I13" s="4">
-        <v>7</v>
-      </c>
-      <c r="J13" s="4">
-        <v>7</v>
-      </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:16384">
+    <row r="14" spans="1:16383">
       <c r="A14" s="1"/>
-      <c r="B14" s="3" t="s">
-        <v>14</v>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>20</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>17</v>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>3</v>
       </c>
-      <c r="F14" s="4">
-        <v>3</v>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3">
+        <v>1</v>
       </c>
-      <c r="G14" s="4">
-        <v>3</v>
+      <c r="J14" s="3">
+        <v>0</v>
       </c>
-      <c r="H14" s="4">
-        <v>3</v>
-      </c>
-      <c r="I14" s="4">
-        <v>3</v>
-      </c>
-      <c r="J14" s="4">
-        <v>3</v>
-      </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:16384">
+    <row r="15" spans="1:16383">
       <c r="A15" s="1"/>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>26</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>18</v>
+      <c r="E15" s="3">
+        <v>5</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>24</v>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3">
+        <v>4</v>
       </c>
-      <c r="E15" s="4">
-        <v>8</v>
+      <c r="K15" s="3">
+        <v>0</v>
       </c>
-      <c r="F15" s="4">
-        <v>8</v>
-      </c>
-      <c r="G15" s="4">
-        <v>8</v>
-      </c>
-      <c r="H15" s="4">
-        <v>8</v>
-      </c>
-      <c r="I15" s="4">
-        <v>8</v>
-      </c>
-      <c r="J15" s="4">
-        <v>8</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:16384">
+    <row r="16" spans="1:16383">
       <c r="A16" s="1"/>
-      <c r="B16" s="3" t="s">
-        <v>14</v>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="D16" s="2" t="s">
+        <v>23</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>25</v>
+      <c r="E16" s="3">
+        <v>8</v>
       </c>
-      <c r="E16" s="4">
-        <v>6</v>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3">
+        <v>7</v>
       </c>
-      <c r="F16" s="4">
-        <v>6</v>
-      </c>
-      <c r="G16" s="4">
-        <v>6</v>
-      </c>
-      <c r="H16" s="4">
-        <v>6</v>
-      </c>
-      <c r="I16" s="4">
-        <v>6</v>
-      </c>
-      <c r="J16" s="4">
-        <v>6</v>
-      </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="1"/>
-      <c r="B17" s="3" t="s">
-        <v>14</v>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>24</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>8</v>
       </c>
-      <c r="F17" s="4">
-        <v>8</v>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3">
+        <v>7</v>
       </c>
-      <c r="G17" s="4">
-        <v>8</v>
-      </c>
-      <c r="H17" s="4">
-        <v>8</v>
-      </c>
-      <c r="I17" s="4">
-        <v>8</v>
-      </c>
-      <c r="J17" s="4">
-        <v>8</v>
-      </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="1"/>
-      <c r="B18" s="3" t="s">
-        <v>14</v>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>25</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="4">
-        <v>9</v>
-      </c>
-      <c r="F18" s="4">
-        <v>9</v>
-      </c>
-      <c r="G18" s="4">
-        <v>9</v>
-      </c>
-      <c r="H18" s="4">
-        <v>9</v>
-      </c>
-      <c r="I18" s="4">
-        <v>9</v>
-      </c>
-      <c r="J18" s="4">
-        <v>9</v>
-      </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="1"/>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="4">
-        <f>SUM(E6:E18)</f>
-        <v>75</v>
+      <c r="E19" s="3">
+        <v>8</v>
       </c>
-      <c r="F19" s="4">
-        <f>E19-$E$19/10</f>
-        <v>67.5</v>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3">
+        <v>7</v>
       </c>
-      <c r="G19" s="4">
-        <f t="shared" ref="G19:O19" si="0">F19-$E$19/10</f>
-        <v>60</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="0"/>
-        <v>52.5</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="J19" s="4">
-        <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-      <c r="K19" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="L19" s="4">
-        <f t="shared" si="0"/>
-        <v>22.5</v>
-      </c>
-      <c r="M19" s="4">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="N19" s="4">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-      <c r="O19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="1"/>
-      <c r="B20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="4">
-        <f>SUM(E6:E18)</f>
-        <v>75</v>
-      </c>
-      <c r="F20" s="4">
-        <f t="shared" ref="F20:J20" si="1">SUM(F6:F18)</f>
-        <v>74</v>
-      </c>
-      <c r="G20" s="4">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="H20" s="4">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="J20" s="4">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
+      <c r="B28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="3">
+        <f>SUM(E6:E27)</f>
+        <v>57</v>
+      </c>
+      <c r="F28" s="3">
+        <f>E28-$E$28/10</f>
+        <v>51.3</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" ref="G28:Q28" si="0">F28-$E$28/10</f>
+        <v>45.599999999999994</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="0"/>
+        <v>39.899999999999991</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="0"/>
+        <v>34.199999999999989</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="0"/>
+        <v>28.499999999999989</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="0"/>
+        <v>22.79999999999999</v>
+      </c>
+      <c r="L28" s="3">
+        <f t="shared" si="0"/>
+        <v>17.099999999999991</v>
+      </c>
+      <c r="M28" s="3">
+        <f t="shared" si="0"/>
+        <v>11.399999999999991</v>
+      </c>
+      <c r="N28" s="3">
+        <f t="shared" si="0"/>
+        <v>5.6999999999999913</v>
+      </c>
+      <c r="O28" s="3">
+        <f t="shared" si="0"/>
+        <v>-8.8817841970012523E-15</v>
+      </c>
+      <c r="P28" s="3">
+        <f t="shared" si="0"/>
+        <v>-5.7000000000000091</v>
+      </c>
+      <c r="Q28" s="3">
+        <f t="shared" si="0"/>
+        <v>-11.400000000000009</v>
+      </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
+      <c r="B29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="3">
+        <f>SUM(E6:E27)</f>
+        <v>57</v>
+      </c>
+      <c r="F29" s="3">
+        <f>SUM(F6:F27)</f>
+        <v>18</v>
+      </c>
+      <c r="G29" s="3">
+        <f>SUM(G6:G27)</f>
+        <v>11</v>
+      </c>
+      <c r="H29" s="3">
+        <f>SUM(H6:H27)</f>
+        <v>4</v>
+      </c>
+      <c r="I29" s="3">
+        <f>SUM(I6:I27)</f>
+        <v>15</v>
+      </c>
+      <c r="J29" s="3">
+        <f>SUM(J6:J27)</f>
+        <v>4</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
@@ -51507,11 +51360,200 @@
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
     </row>
+    <row r="57" spans="1:19">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+    </row>
+    <row r="58" spans="1:19">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+    </row>
+    <row r="59" spans="1:19">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+    </row>
+    <row r="60" spans="1:19">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+    </row>
+    <row r="61" spans="1:19">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+    </row>
+    <row r="62" spans="1:19">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+    </row>
+    <row r="63" spans="1:19">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+    </row>
+    <row r="64" spans="1:19">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+    </row>
+    <row r="65" spans="1:19">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+    </row>
   </sheetData>
   <sheetProtection password="EF56" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="E1:H1"/>
   </mergeCells>

</xml_diff>

<commit_message>
rapikan slide, tambah strabismus
</commit_message>
<xml_diff>
--- a/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
+++ b/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Project</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>9 Hewan Albino Terindah</t>
+  </si>
+  <si>
+    <t>Persilangan Albino</t>
+  </si>
+  <si>
+    <t>persilangan pada albino</t>
   </si>
 </sst>
 </file>
@@ -297,7 +303,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="id-ID"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -315,7 +321,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -335,7 +340,7 @@
                 <a:pPr>
                   <a:defRPr lang="en-US"/>
                 </a:pPr>
-                <a:endParaRPr lang="id-ID"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showVal val="1"/>
@@ -386,34 +391,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>51.3</c:v>
+                  <c:v>71.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.599999999999994</c:v>
+                  <c:v>63.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.899999999999991</c:v>
+                  <c:v>55.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.199999999999989</c:v>
+                  <c:v>47.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.499999999999989</c:v>
+                  <c:v>39.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.79999999999999</c:v>
+                  <c:v>31.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.099999999999991</c:v>
+                  <c:v>23.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.399999999999991</c:v>
+                  <c:v>15.800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.6999999999999913</c:v>
+                  <c:v>7.9000000000000021</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-8.8817841970012523E-15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -433,7 +438,7 @@
                 <a:pPr>
                   <a:defRPr lang="en-US"/>
                 </a:pPr>
-                <a:endParaRPr lang="id-ID"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showVal val="1"/>
@@ -484,10 +489,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -498,6 +503,12 @@
                 <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -506,11 +517,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="70381952"/>
-        <c:axId val="70383488"/>
+        <c:axId val="60080512"/>
+        <c:axId val="60082048"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="70381952"/>
+        <c:axId val="60080512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -525,16 +536,16 @@
             <a:pPr>
               <a:defRPr lang="en-US"/>
             </a:pPr>
-            <a:endParaRPr lang="id-ID"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70383488"/>
+        <c:crossAx val="60082048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="70383488"/>
+        <c:axId val="60082048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,14 +553,13 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="70381952"/>
+        <c:crossAx val="60080512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -557,7 +567,7 @@
           <a:pPr>
             <a:defRPr lang="en-US"/>
           </a:pPr>
-          <a:endParaRPr lang="id-ID"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -565,7 +575,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -894,7 +904,7 @@
   <dimension ref="A1:XFC65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -50149,10 +50159,18 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="E6" s="3">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3">
+        <v>6</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -50172,10 +50190,18 @@
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="E7" s="3">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -50207,7 +50233,9 @@
       <c r="H8" s="3">
         <v>2</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -50238,7 +50266,9 @@
       <c r="H9" s="3">
         <v>1</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -50342,7 +50372,9 @@
       <c r="H13" s="3">
         <v>1</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -50513,7 +50545,9 @@
       <c r="K19" s="3">
         <v>7</v>
       </c>
-      <c r="L19" s="3"/>
+      <c r="L19" s="3">
+        <v>1</v>
+      </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -50525,16 +50559,24 @@
     <row r="20" spans="1:19">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="3">
+        <v>8</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="L20" s="3">
+        <v>5</v>
+      </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -50699,55 +50741,55 @@
       <c r="D28" s="8"/>
       <c r="E28" s="3">
         <f>SUM(E6:E27)</f>
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="F28" s="3">
         <f>E28-$E$28/10</f>
-        <v>51.3</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" ref="G28:Q28" si="0">F28-$E$28/10</f>
-        <v>45.599999999999994</v>
+        <v>63.199999999999996</v>
       </c>
       <c r="H28" s="3">
         <f t="shared" si="0"/>
-        <v>39.899999999999991</v>
+        <v>55.3</v>
       </c>
       <c r="I28" s="3">
         <f t="shared" si="0"/>
-        <v>34.199999999999989</v>
+        <v>47.4</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" si="0"/>
-        <v>28.499999999999989</v>
+        <v>39.5</v>
       </c>
       <c r="K28" s="3">
         <f t="shared" si="0"/>
-        <v>22.79999999999999</v>
+        <v>31.6</v>
       </c>
       <c r="L28" s="3">
         <f t="shared" si="0"/>
-        <v>17.099999999999991</v>
+        <v>23.700000000000003</v>
       </c>
       <c r="M28" s="3">
         <f t="shared" si="0"/>
-        <v>11.399999999999991</v>
+        <v>15.800000000000002</v>
       </c>
       <c r="N28" s="3">
         <f t="shared" si="0"/>
-        <v>5.6999999999999913</v>
+        <v>7.9000000000000021</v>
       </c>
       <c r="O28" s="3">
         <f t="shared" si="0"/>
-        <v>-8.8817841970012523E-15</v>
+        <v>0</v>
       </c>
       <c r="P28" s="3">
         <f t="shared" si="0"/>
-        <v>-5.7000000000000091</v>
+        <v>-7.9</v>
       </c>
       <c r="Q28" s="3">
         <f t="shared" si="0"/>
-        <v>-11.400000000000009</v>
+        <v>-15.8</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -50760,31 +50802,35 @@
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="3">
-        <f>SUM(E6:E27)</f>
-        <v>57</v>
+        <f t="shared" ref="E29:J29" si="1">SUM(E6:E27)</f>
+        <v>79</v>
       </c>
       <c r="F29" s="3">
-        <f>SUM(F6:F27)</f>
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>29</v>
       </c>
       <c r="G29" s="3">
-        <f>SUM(G6:G27)</f>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="H29" s="3">
-        <f>SUM(H6:H27)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I29" s="3">
-        <f>SUM(I6:I27)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="J29" s="3">
-        <f>SUM(J6:J27)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="K29" s="3">
+        <v>7</v>
+      </c>
+      <c r="L29" s="3">
+        <v>6</v>
+      </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>

</xml_diff>

<commit_message>
rapikan slide dan tambah style
</commit_message>
<xml_diff>
--- a/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
+++ b/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Project</t>
   </si>
@@ -156,7 +156,34 @@
     <t>Persilangan Albino</t>
   </si>
   <si>
-    <t>persilangan pada albino</t>
+    <t>Persilangan Pada Albino</t>
+  </si>
+  <si>
+    <t>Kelainan Mata Albino</t>
+  </si>
+  <si>
+    <t>Nystagmus</t>
+  </si>
+  <si>
+    <t>Strabismus</t>
+  </si>
+  <si>
+    <t>Mata Silindris (Astigmatism)</t>
+  </si>
+  <si>
+    <t>Albino Pada Tanaman</t>
+  </si>
+  <si>
+    <t>Reed Wood Tree Albino</t>
+  </si>
+  <si>
+    <t>Albino Pada Tanaman Jagung</t>
+  </si>
+  <si>
+    <t>Ambliopia</t>
+  </si>
+  <si>
+    <t>Fotophobia</t>
   </si>
 </sst>
 </file>
@@ -321,6 +348,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -391,31 +419,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>71.099999999999994</c:v>
+                  <c:v>142.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.199999999999996</c:v>
+                  <c:v>126.39999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.3</c:v>
+                  <c:v>110.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47.4</c:v>
+                  <c:v>94.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.5</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.6</c:v>
+                  <c:v>63.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.700000000000003</c:v>
+                  <c:v>47.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.800000000000002</c:v>
+                  <c:v>31.600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.9000000000000021</c:v>
+                  <c:v>15.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -489,25 +517,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -517,11 +551,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="60080512"/>
-        <c:axId val="60082048"/>
+        <c:axId val="65200512"/>
+        <c:axId val="65202048"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="60080512"/>
+        <c:axId val="65200512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,13 +573,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60082048"/>
+        <c:crossAx val="65202048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="60082048"/>
+        <c:axId val="65202048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,13 +587,14 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="60080512"/>
+        <c:crossAx val="65200512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -575,7 +610,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -903,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -50163,14 +50198,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="3">
-        <v>6</v>
-      </c>
-      <c r="G6" s="3">
         <v>0</v>
       </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -50197,11 +50228,9 @@
         <v>5</v>
       </c>
       <c r="G7" s="3">
-        <v>3</v>
-      </c>
-      <c r="H7" s="3">
         <v>0</v>
       </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -50289,9 +50318,13 @@
       <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <v>8</v>
+      </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -50312,9 +50345,13 @@
       <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3">
+        <v>7</v>
+      </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -50337,9 +50374,13 @@
       <c r="D12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3">
+        <v>6</v>
+      </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -50509,14 +50550,24 @@
       <c r="D18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3">
+        <v>8</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="I18" s="3">
+        <v>4</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -50548,7 +50599,9 @@
       <c r="L19" s="3">
         <v>1</v>
       </c>
-      <c r="M19" s="3"/>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
@@ -50575,7 +50628,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -50588,16 +50641,24 @@
     <row r="21" spans="1:19">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
+      <c r="C21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="3">
+        <v>6</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -50610,8 +50671,12 @@
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -50619,8 +50684,12 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
+      <c r="M22" s="3">
+        <v>6</v>
+      </c>
+      <c r="N22" s="3">
+        <v>2</v>
+      </c>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -50631,8 +50700,12 @@
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="3">
+        <v>7</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -50641,7 +50714,9 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+      <c r="N23" s="3">
+        <v>2</v>
+      </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -50652,8 +50727,12 @@
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="3">
+        <v>7</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -50661,8 +50740,12 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
+      <c r="M24" s="3">
+        <v>6</v>
+      </c>
+      <c r="N24" s="3">
+        <v>0</v>
+      </c>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -50673,8 +50756,12 @@
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="3">
+        <v>8</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -50683,7 +50770,9 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="N25" s="3">
+        <v>3</v>
+      </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -50693,9 +50782,15 @@
     <row r="26" spans="1:19">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
+      <c r="C26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="3">
+        <v>8</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -50703,8 +50798,12 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
+      <c r="M26" s="3">
+        <v>3</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0</v>
+      </c>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -50715,8 +50814,12 @@
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
+      <c r="D27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="3">
+        <v>6</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -50724,8 +50827,12 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="M27" s="3">
+        <v>3</v>
+      </c>
+      <c r="N27" s="3">
+        <v>0</v>
+      </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
@@ -50741,43 +50848,43 @@
       <c r="D28" s="8"/>
       <c r="E28" s="3">
         <f>SUM(E6:E27)</f>
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="F28" s="3">
         <f>E28-$E$28/10</f>
-        <v>71.099999999999994</v>
+        <v>142.19999999999999</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" ref="G28:Q28" si="0">F28-$E$28/10</f>
-        <v>63.199999999999996</v>
+        <v>126.39999999999999</v>
       </c>
       <c r="H28" s="3">
         <f t="shared" si="0"/>
-        <v>55.3</v>
+        <v>110.6</v>
       </c>
       <c r="I28" s="3">
         <f t="shared" si="0"/>
-        <v>47.4</v>
+        <v>94.8</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" si="0"/>
-        <v>39.5</v>
+        <v>79</v>
       </c>
       <c r="K28" s="3">
         <f t="shared" si="0"/>
-        <v>31.6</v>
+        <v>63.2</v>
       </c>
       <c r="L28" s="3">
         <f t="shared" si="0"/>
-        <v>23.700000000000003</v>
+        <v>47.400000000000006</v>
       </c>
       <c r="M28" s="3">
         <f t="shared" si="0"/>
-        <v>15.800000000000002</v>
+        <v>31.600000000000005</v>
       </c>
       <c r="N28" s="3">
         <f t="shared" si="0"/>
-        <v>7.9000000000000021</v>
+        <v>15.800000000000004</v>
       </c>
       <c r="O28" s="3">
         <f t="shared" si="0"/>
@@ -50785,11 +50892,11 @@
       </c>
       <c r="P28" s="3">
         <f t="shared" si="0"/>
-        <v>-7.9</v>
+        <v>-15.8</v>
       </c>
       <c r="Q28" s="3">
         <f t="shared" si="0"/>
-        <v>-15.8</v>
+        <v>-31.6</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -50803,15 +50910,15 @@
       <c r="D29" s="8"/>
       <c r="E29" s="3">
         <f t="shared" ref="E29:J29" si="1">SUM(E6:E27)</f>
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="1"/>
@@ -50819,20 +50926,28 @@
       </c>
       <c r="I29" s="3">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K29" s="3">
+        <f>SUM(K6:K27)</f>
+        <v>8</v>
+      </c>
+      <c r="L29" s="3">
+        <f>SUM(L6:L27)</f>
+        <v>1</v>
+      </c>
+      <c r="M29" s="3">
+        <f>SUM(M6:M27)</f>
+        <v>18</v>
+      </c>
+      <c r="N29" s="3">
+        <f t="shared" ref="N29:Q29" si="2">SUM(N6:N27)</f>
         <v>7</v>
       </c>
-      <c r="L29" s="3">
-        <v>6</v>
-      </c>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>

</xml_diff>

<commit_message>
rapikan dan tambah style slide albino hewan
</commit_message>
<xml_diff>
--- a/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
+++ b/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Project</t>
   </si>
@@ -156,40 +156,34 @@
     <t>Persilangan Albino</t>
   </si>
   <si>
-    <t>persilangan pada albino</t>
+    <t>Persilangan Pada Albino</t>
   </si>
   <si>
-    <t>Tantangan Sosial</t>
+    <t>Kelainan Mata Albino</t>
   </si>
   <si>
-    <t>Tantangan sosial penderita albino</t>
+    <t>Nystagmus</t>
   </si>
   <si>
-    <t>Legenda Albino di Indonesia</t>
+    <t>Strabismus</t>
   </si>
   <si>
-    <t>Albino di desa Mantar</t>
+    <t>Mata Silindris (Astigmatism)</t>
   </si>
   <si>
     <t>Albino Pada Tanaman</t>
   </si>
   <si>
-    <t>Albino pada tanaman jagung</t>
+    <t>Reed Wood Tree Albino</t>
   </si>
   <si>
-    <t>Albino pada Redwood Tree</t>
+    <t>Albino Pada Tanaman Jagung</t>
   </si>
   <si>
-    <t>Kelainan Mata pada Albino</t>
+    <t>Ambliopia</t>
   </si>
   <si>
-    <t>Mata Silindris</t>
-  </si>
-  <si>
-    <t>Fotofobia</t>
-  </si>
-  <si>
-    <t>Strabismus</t>
+    <t>Fotophobia</t>
   </si>
 </sst>
 </file>
@@ -336,7 +330,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="id-ID"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -374,7 +368,7 @@
                 <a:pPr>
                   <a:defRPr lang="en-US"/>
                 </a:pPr>
-                <a:endParaRPr lang="id-ID"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showVal val="1"/>
@@ -425,31 +419,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>103.5</c:v>
+                  <c:v>142.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92</c:v>
+                  <c:v>126.39999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.5</c:v>
+                  <c:v>110.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>69</c:v>
+                  <c:v>94.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57.5</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46</c:v>
+                  <c:v>63.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.5</c:v>
+                  <c:v>47.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>31.600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.5</c:v>
+                  <c:v>15.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -472,7 +466,7 @@
                 <a:pPr>
                   <a:defRPr lang="en-US"/>
                 </a:pPr>
-                <a:endParaRPr lang="id-ID"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showVal val="1"/>
@@ -523,25 +517,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>23</c:v>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -551,11 +551,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="57757696"/>
-        <c:axId val="57759232"/>
+        <c:axId val="65200512"/>
+        <c:axId val="65202048"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="57757696"/>
+        <c:axId val="65200512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -570,16 +570,16 @@
             <a:pPr>
               <a:defRPr lang="en-US"/>
             </a:pPr>
-            <a:endParaRPr lang="id-ID"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57759232"/>
+        <c:crossAx val="65202048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="57759232"/>
+        <c:axId val="65202048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,7 +587,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="57757696"/>
+        <c:crossAx val="65200512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -602,7 +602,7 @@
           <a:pPr>
             <a:defRPr lang="en-US"/>
           </a:pPr>
-          <a:endParaRPr lang="id-ID"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -610,7 +610,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -938,14 +938,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="34.140625" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
@@ -50198,14 +50198,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="3">
-        <v>6</v>
-      </c>
-      <c r="G6" s="3">
         <v>0</v>
       </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -50232,11 +50228,9 @@
         <v>5</v>
       </c>
       <c r="G7" s="3">
-        <v>3</v>
-      </c>
-      <c r="H7" s="3">
         <v>0</v>
       </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -50325,18 +50319,14 @@
         <v>15</v>
       </c>
       <c r="E10" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3">
         <v>0</v>
       </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -50356,18 +50346,14 @@
         <v>16</v>
       </c>
       <c r="E11" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3">
         <v>0</v>
       </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -50391,15 +50377,11 @@
       <c r="E12" s="3">
         <v>6</v>
       </c>
-      <c r="F12" s="3">
-        <v>3</v>
-      </c>
+      <c r="F12" s="3"/>
       <c r="G12" s="3">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3">
         <v>0</v>
       </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -50568,14 +50550,24 @@
       <c r="D18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3">
+        <v>8</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="I18" s="3">
+        <v>4</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -50607,7 +50599,9 @@
       <c r="L19" s="3">
         <v>1</v>
       </c>
-      <c r="M19" s="3"/>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
@@ -50634,7 +50628,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -50654,29 +50648,19 @@
         <v>32</v>
       </c>
       <c r="E21" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3">
-        <v>8</v>
-      </c>
-      <c r="J21" s="3">
-        <v>5</v>
-      </c>
-      <c r="K21" s="3">
-        <v>3</v>
-      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
       <c r="L21" s="3">
-        <v>2</v>
-      </c>
-      <c r="M21" s="3">
-        <v>1</v>
-      </c>
-      <c r="N21" s="3">
         <v>0</v>
       </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -50686,30 +50670,26 @@
     <row r="22" spans="1:19">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="E22" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="3">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3">
+        <v>6</v>
+      </c>
+      <c r="N22" s="3">
         <v>2</v>
       </c>
-      <c r="K22" s="3">
-        <v>2</v>
-      </c>
-      <c r="L22" s="3">
-        <v>0</v>
-      </c>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -50719,14 +50699,12 @@
     <row r="23" spans="1:19">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E23" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -50735,11 +50713,9 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="3">
+      <c r="M23" s="3"/>
+      <c r="N23" s="3">
         <v>2</v>
-      </c>
-      <c r="N23" s="3">
-        <v>0</v>
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -50752,10 +50728,10 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E24" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -50764,13 +50740,13 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="M24" s="3">
+        <v>6</v>
+      </c>
       <c r="N24" s="3">
-        <v>2</v>
-      </c>
-      <c r="O24" s="3">
         <v>0</v>
       </c>
+      <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="1"/>
@@ -50779,13 +50755,13 @@
     <row r="25" spans="1:19">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>39</v>
+      <c r="E25" s="3">
+        <v>8</v>
       </c>
-      <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -50794,7 +50770,9 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="N25" s="3">
+        <v>3</v>
+      </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -50804,11 +50782,15 @@
     <row r="26" spans="1:19">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D26" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="3">
+        <v>8</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -50816,8 +50798,12 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
+      <c r="M26" s="3">
+        <v>3</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0</v>
+      </c>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -50829,9 +50815,11 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="3">
+        <v>6</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -50839,8 +50827,12 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="M27" s="3">
+        <v>3</v>
+      </c>
+      <c r="N27" s="3">
+        <v>0</v>
+      </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
@@ -50856,43 +50848,43 @@
       <c r="D28" s="8"/>
       <c r="E28" s="3">
         <f>SUM(E6:E27)</f>
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="F28" s="3">
         <f>E28-$E$28/10</f>
-        <v>103.5</v>
+        <v>142.19999999999999</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" ref="G28:Q28" si="0">F28-$E$28/10</f>
-        <v>92</v>
+        <v>126.39999999999999</v>
       </c>
       <c r="H28" s="3">
         <f t="shared" si="0"/>
-        <v>80.5</v>
+        <v>110.6</v>
       </c>
       <c r="I28" s="3">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>94.8</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" si="0"/>
-        <v>57.5</v>
+        <v>79</v>
       </c>
       <c r="K28" s="3">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>63.2</v>
       </c>
       <c r="L28" s="3">
         <f t="shared" si="0"/>
-        <v>34.5</v>
+        <v>47.400000000000006</v>
       </c>
       <c r="M28" s="3">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>31.600000000000005</v>
       </c>
       <c r="N28" s="3">
         <f t="shared" si="0"/>
-        <v>11.5</v>
+        <v>15.800000000000004</v>
       </c>
       <c r="O28" s="3">
         <f t="shared" si="0"/>
@@ -50900,11 +50892,11 @@
       </c>
       <c r="P28" s="3">
         <f t="shared" si="0"/>
-        <v>-11.5</v>
+        <v>-15.8</v>
       </c>
       <c r="Q28" s="3">
         <f t="shared" si="0"/>
-        <v>-23</v>
+        <v>-31.6</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -50918,36 +50910,44 @@
       <c r="D29" s="8"/>
       <c r="E29" s="3">
         <f t="shared" ref="E29:J29" si="1">SUM(E6:E27)</f>
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I29" s="3">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K29" s="3">
+        <f>SUM(K6:K27)</f>
+        <v>8</v>
+      </c>
+      <c r="L29" s="3">
+        <f>SUM(L6:L27)</f>
+        <v>1</v>
+      </c>
+      <c r="M29" s="3">
+        <f>SUM(M6:M27)</f>
+        <v>18</v>
+      </c>
+      <c r="N29" s="3">
+        <f t="shared" ref="N29:Q29" si="2">SUM(N6:N27)</f>
         <v>7</v>
       </c>
-      <c r="L29" s="3">
-        <v>6</v>
-      </c>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>

</xml_diff>

<commit_message>
adit slide, tambah background dan tambah style
</commit_message>
<xml_diff>
--- a/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
+++ b/public/Log Book dan BurnDownChart/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Project</t>
   </si>
@@ -156,58 +156,34 @@
     <t>Persilangan Albino</t>
   </si>
   <si>
-    <t>persilangan pada albino</t>
+    <t>Persilangan Pada Albino</t>
   </si>
   <si>
-    <t>Tantangan Sosial</t>
+    <t>Kelainan Mata Albino</t>
   </si>
   <si>
-    <t>Tantangan sosial penderita albino</t>
+    <t>Nystagmus</t>
   </si>
   <si>
-    <t>Legenda Albino di Indonesia</t>
+    <t>Strabismus</t>
   </si>
   <si>
-    <t>Albino di desa Mantar</t>
+    <t>Mata Silindris (Astigmatism)</t>
   </si>
   <si>
     <t>Albino Pada Tanaman</t>
   </si>
   <si>
-    <t>Albino pada tanaman jagung</t>
+    <t>Reed Wood Tree Albino</t>
   </si>
   <si>
-    <t>Albino pada Redwood Tree</t>
-  </si>
-  <si>
-    <t>Kelainan Mata pada Albino</t>
-  </si>
-  <si>
-    <t>Mata Silindris</t>
-  </si>
-  <si>
-    <t>Fotofobia</t>
-  </si>
-  <si>
-    <t>Strabismus</t>
-  </si>
-  <si>
-    <t>Nystagmus</t>
+    <t>Albino Pada Tanaman Jagung</t>
   </si>
   <si>
     <t>Ambliopia</t>
   </si>
   <si>
-    <t>Keindahan Alabino pada Manusia</t>
-  </si>
-  <si>
-    <t>Ambliopia Strabismik</t>
-  </si>
-  <si>
-    <t>Ambliopia Anisometric</t>
-  </si>
-  <si>
-    <t>Ambliopia Devripatif</t>
+    <t>Fotophobia</t>
   </si>
 </sst>
 </file>
@@ -354,7 +330,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="id-ID"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -392,7 +368,7 @@
                 <a:pPr>
                   <a:defRPr lang="en-US"/>
                 </a:pPr>
-                <a:endParaRPr lang="id-ID"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showVal val="1"/>
@@ -438,36 +414,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$34:$O$34</c:f>
+              <c:f>Sheet1!$F$28:$O$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>103.5</c:v>
+                  <c:v>142.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92</c:v>
+                  <c:v>126.39999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.5</c:v>
+                  <c:v>110.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>69</c:v>
+                  <c:v>94.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57.5</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46</c:v>
+                  <c:v>63.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.5</c:v>
+                  <c:v>47.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>31.600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.5</c:v>
+                  <c:v>15.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -490,7 +466,7 @@
                 <a:pPr>
                   <a:defRPr lang="en-US"/>
                 </a:pPr>
-                <a:endParaRPr lang="id-ID"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showVal val="1"/>
@@ -536,30 +512,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$35:$O$35</c:f>
+              <c:f>Sheet1!$F$29:$O$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>23</c:v>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -569,11 +551,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="59527168"/>
-        <c:axId val="59528704"/>
+        <c:axId val="65200512"/>
+        <c:axId val="65202048"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="59527168"/>
+        <c:axId val="65200512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -588,16 +570,16 @@
             <a:pPr>
               <a:defRPr lang="en-US"/>
             </a:pPr>
-            <a:endParaRPr lang="id-ID"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59528704"/>
+        <c:crossAx val="65202048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="59528704"/>
+        <c:axId val="65202048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,7 +587,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="59527168"/>
+        <c:crossAx val="65200512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -620,7 +602,7 @@
           <a:pPr>
             <a:defRPr lang="en-US"/>
           </a:pPr>
-          <a:endParaRPr lang="id-ID"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -639,15 +621,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>628651</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>514351</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -956,14 +938,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="34.140625" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
@@ -50216,14 +50198,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="3">
-        <v>6</v>
-      </c>
-      <c r="G6" s="3">
         <v>0</v>
       </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -50250,11 +50228,9 @@
         <v>5</v>
       </c>
       <c r="G7" s="3">
-        <v>3</v>
-      </c>
-      <c r="H7" s="3">
         <v>0</v>
       </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -50343,18 +50319,14 @@
         <v>15</v>
       </c>
       <c r="E10" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3">
         <v>0</v>
       </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -50374,18 +50346,14 @@
         <v>16</v>
       </c>
       <c r="E11" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3">
         <v>0</v>
       </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -50409,15 +50377,11 @@
       <c r="E12" s="3">
         <v>6</v>
       </c>
-      <c r="F12" s="3">
-        <v>3</v>
-      </c>
+      <c r="F12" s="3"/>
       <c r="G12" s="3">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3">
         <v>0</v>
       </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -50586,14 +50550,24 @@
       <c r="D18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3">
+        <v>8</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="I18" s="3">
+        <v>4</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -50625,7 +50599,9 @@
       <c r="L19" s="3">
         <v>1</v>
       </c>
-      <c r="M19" s="3"/>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
@@ -50652,7 +50628,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -50672,29 +50648,19 @@
         <v>32</v>
       </c>
       <c r="E21" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3">
-        <v>8</v>
-      </c>
-      <c r="J21" s="3">
-        <v>5</v>
-      </c>
-      <c r="K21" s="3">
-        <v>3</v>
-      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
       <c r="L21" s="3">
-        <v>2</v>
-      </c>
-      <c r="M21" s="3">
-        <v>1</v>
-      </c>
-      <c r="N21" s="3">
         <v>0</v>
       </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -50704,30 +50670,26 @@
     <row r="22" spans="1:19">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="E22" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="3">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3">
+        <v>6</v>
+      </c>
+      <c r="N22" s="3">
         <v>2</v>
       </c>
-      <c r="K22" s="3">
-        <v>2</v>
-      </c>
-      <c r="L22" s="3">
-        <v>0</v>
-      </c>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -50737,14 +50699,12 @@
     <row r="23" spans="1:19">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E23" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -50753,11 +50713,9 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="3">
+      <c r="M23" s="3"/>
+      <c r="N23" s="3">
         <v>2</v>
-      </c>
-      <c r="N23" s="3">
-        <v>0</v>
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -50770,10 +50728,10 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E24" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -50782,13 +50740,13 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="M24" s="3">
+        <v>6</v>
+      </c>
       <c r="N24" s="3">
-        <v>2</v>
-      </c>
-      <c r="O24" s="3">
         <v>0</v>
       </c>
+      <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="1"/>
@@ -50797,13 +50755,13 @@
     <row r="25" spans="1:19">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>39</v>
+      <c r="E25" s="3">
+        <v>8</v>
       </c>
-      <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -50812,7 +50770,9 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="N25" s="3">
+        <v>3</v>
+      </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -50822,11 +50782,15 @@
     <row r="26" spans="1:19">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D26" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="3">
+        <v>8</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -50834,8 +50798,12 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
+      <c r="M26" s="3">
+        <v>3</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0</v>
+      </c>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -50847,9 +50815,11 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="3">
+        <v>6</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -50857,8 +50827,12 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="M27" s="3">
+        <v>3</v>
+      </c>
+      <c r="N27" s="3">
+        <v>0</v>
+      </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
@@ -50867,44 +50841,113 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>42</v>
+      <c r="B28" s="8" t="s">
+        <v>4</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="3">
+        <f>SUM(E6:E27)</f>
+        <v>158</v>
+      </c>
+      <c r="F28" s="3">
+        <f>E28-$E$28/10</f>
+        <v>142.19999999999999</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" ref="G28:Q28" si="0">F28-$E$28/10</f>
+        <v>126.39999999999999</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="0"/>
+        <v>110.6</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="0"/>
+        <v>94.8</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="0"/>
+        <v>63.2</v>
+      </c>
+      <c r="L28" s="3">
+        <f t="shared" si="0"/>
+        <v>47.400000000000006</v>
+      </c>
+      <c r="M28" s="3">
+        <f t="shared" si="0"/>
+        <v>31.600000000000005</v>
+      </c>
+      <c r="N28" s="3">
+        <f t="shared" si="0"/>
+        <v>15.800000000000004</v>
+      </c>
+      <c r="O28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="3">
+        <f t="shared" si="0"/>
+        <v>-15.8</v>
+      </c>
+      <c r="Q28" s="3">
+        <f t="shared" si="0"/>
+        <v>-31.6</v>
+      </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19">
       <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
-        <v>43</v>
+      <c r="B29" s="8" t="s">
+        <v>5</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="3">
+        <f t="shared" ref="E29:J29" si="1">SUM(E6:E27)</f>
+        <v>158</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K29" s="3">
+        <f>SUM(K6:K27)</f>
+        <v>8</v>
+      </c>
+      <c r="L29" s="3">
+        <f>SUM(L6:L27)</f>
+        <v>1</v>
+      </c>
+      <c r="M29" s="3">
+        <f>SUM(M6:M27)</f>
+        <v>18</v>
+      </c>
+      <c r="N29" s="3">
+        <f t="shared" ref="N29:Q29" si="2">SUM(N6:N27)</f>
+        <v>7</v>
+      </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
@@ -50913,204 +50956,127 @@
     </row>
     <row r="30" spans="1:19">
       <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19">
       <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19">
       <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19">
       <c r="A34" s="1"/>
-      <c r="B34" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="3">
-        <f>SUM(E6:E27)</f>
-        <v>115</v>
-      </c>
-      <c r="F34" s="3">
-        <f>E34-$E$34/10</f>
-        <v>103.5</v>
-      </c>
-      <c r="G34" s="3">
-        <f>F34-$E$34/10</f>
-        <v>92</v>
-      </c>
-      <c r="H34" s="3">
-        <f>G34-$E$34/10</f>
-        <v>80.5</v>
-      </c>
-      <c r="I34" s="3">
-        <f>H34-$E$34/10</f>
-        <v>69</v>
-      </c>
-      <c r="J34" s="3">
-        <f>I34-$E$34/10</f>
-        <v>57.5</v>
-      </c>
-      <c r="K34" s="3">
-        <f>J34-$E$34/10</f>
-        <v>46</v>
-      </c>
-      <c r="L34" s="3">
-        <f>K34-$E$34/10</f>
-        <v>34.5</v>
-      </c>
-      <c r="M34" s="3">
-        <f>L34-$E$34/10</f>
-        <v>23</v>
-      </c>
-      <c r="N34" s="3">
-        <f>M34-$E$34/10</f>
-        <v>11.5</v>
-      </c>
-      <c r="O34" s="3">
-        <f>N34-$E$34/10</f>
-        <v>0</v>
-      </c>
-      <c r="P34" s="3">
-        <f>O34-$E$34/10</f>
-        <v>-11.5</v>
-      </c>
-      <c r="Q34" s="3">
-        <f>P34-$E$34/10</f>
-        <v>-23</v>
-      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19">
       <c r="A35" s="1"/>
-      <c r="B35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="3">
-        <f>SUM(E6:E27)</f>
-        <v>115</v>
-      </c>
-      <c r="F35" s="3">
-        <f>SUM(F6:F27)</f>
-        <v>32</v>
-      </c>
-      <c r="G35" s="3">
-        <f>SUM(G6:G27)</f>
-        <v>19</v>
-      </c>
-      <c r="H35" s="3">
-        <f>SUM(H6:H27)</f>
-        <v>8</v>
-      </c>
-      <c r="I35" s="3">
-        <f>SUM(I6:I27)</f>
-        <v>23</v>
-      </c>
-      <c r="J35" s="3">
-        <f>SUM(J6:J27)</f>
-        <v>11</v>
-      </c>
-      <c r="K35" s="3">
-        <v>7</v>
-      </c>
-      <c r="L35" s="3">
-        <v>6</v>
-      </c>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
@@ -51747,8 +51713,8 @@
   </sheetData>
   <sheetProtection password="EF56" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="E1:H1"/>
   </mergeCells>

</xml_diff>